<commit_message>
added library in the requierments
</commit_message>
<xml_diff>
--- a/Sales_Conversation_Twilio.xlsx
+++ b/Sales_Conversation_Twilio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,13 +1399,189 @@
           <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it.</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>45964.77464993056</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>45964.78596905093</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Yes.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>45964.78619211805</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>45964.78638554398</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>45964.82465596065</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>45964.82489373843</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Uh, just not interested.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>45964.82510863426</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>+917990747606</t>
         </is>
       </c>
-      <c r="F35" s="2" t="n">
-        <v>45964.77464992835</v>
+      <c r="F42" s="2" t="n">
+        <v>45964.82681271759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented calling from the execl sheet and saving the data from the excel sheet
</commit_message>
<xml_diff>
--- a/Sales_Conversation_Twilio.xlsx
+++ b/Sales_Conversation_Twilio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1575,13 +1575,418 @@
           <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>+917990747606</t>
-        </is>
+      <c r="E42" t="n">
+        <v>917990747606</v>
       </c>
       <c r="F42" s="2" t="n">
-        <v>45964.82681271759</v>
+        <v>45964.8268127199</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F43" s="2" t="n">
+        <v>45965.82953266204</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No, not interested.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F44" s="2" t="n">
+        <v>45965.82975902778</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F45" s="2" t="n">
+        <v>45965.82994740741</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>90.  Can I put you on?</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F46" s="2" t="n">
+        <v>45965.83004488426</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Thank you.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F47" s="2" t="n">
+        <v>45965.83013833333</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Take.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F48" s="2" t="n">
+        <v>45965.83021</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F49" s="2" t="n">
+        <v>45965.83035658565</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F50" s="2" t="n">
+        <v>45965.83057212963</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>No.</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F51" s="2" t="n">
+        <v>45965.83076421297</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Number.</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F52" s="2" t="n">
+        <v>45965.83084753472</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Hello.  I,</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F53" s="2" t="n">
+        <v>45965.83104321759</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>[Agent check]</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Talk to agent.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Our agent will contact you later. Meanwhile, would you like to hear about our products?</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F54" s="2" t="n">
+        <v>45965.83141940973</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Your voice.  yeah, but</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F55" s="2" t="n">
+        <v>45965.8316612963</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>+919510038048</t>
+        </is>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>45965.83205196181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented the supabase and refiended
</commit_message>
<xml_diff>
--- a/Sales_Conversation_Twilio.xlsx
+++ b/Sales_Conversation_Twilio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1980,13 +1980,475 @@
           <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="E56" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F56" s="2" t="n">
+        <v>45965.83205196759</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Good afternoon! I am your sales agent from Creer Infotech. Would you like to hear about our latest products?</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F57" s="2" t="n">
+        <v>45967.56912234954</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F58" s="2" t="n">
+        <v>45972.81882967593</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Yes, I am still  there.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F59" s="2" t="n">
+        <v>45972.81929960648</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Yes Bank</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F60" s="2" t="n">
+        <v>45972.819420625</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>none of the above no</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F61" s="2" t="n">
+        <v>45972.81985011574</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Hai yes, I am there right here.  Yes, I am there right  here.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F62" s="2" t="n">
+        <v>45972.82033612268</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Yas Bluetooth earbuds?</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F63" s="2" t="n">
+        <v>45972.82086135416</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F64" s="2" t="n">
+        <v>45975.55740662037</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>I M stil deyar. Hello I am speaking.</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F65" s="2" t="n">
+        <v>45975.55791690973</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F66" s="2" t="n">
+        <v>45975.55824385417</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F67" s="2" t="n">
+        <v>45986.76252136574</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>[Persuasion check]</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>no no no</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F68" s="2" t="n">
+        <v>45986.76287478009</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>yas yas</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F69" s="2" t="n">
+        <v>45986.76332363426</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>laptop Pro</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Laptop Pro  to your phone number ending with 7606. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>917990747606</v>
+      </c>
+      <c r="F70" s="2" t="n">
+        <v>45986.76354986111</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F71" s="2" t="n">
+        <v>45987.63015055555</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Yes.</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F72" s="2" t="n">
+        <v>45987.63036466435</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
         <is>
           <t>+919510038048</t>
         </is>
       </c>
-      <c r="F56" s="2" t="n">
-        <v>45965.83205196181</v>
+      <c r="F73" s="2" t="n">
+        <v>45987.63049465394</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made resolved the code and made the code working
</commit_message>
<xml_diff>
--- a/Sales_Conversation_Twilio.xlsx
+++ b/Sales_Conversation_Twilio.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2442,13 +2442,264 @@
           <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E73" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F73" s="2" t="n">
+        <v>45987.63049465277</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F74" s="2" t="n">
+        <v>45988.66858461806</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F75" s="2" t="n">
+        <v>45988.6697115625</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F76" s="2" t="n">
+        <v>45988.67003817129</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Bluetooth earphones</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F77" s="2" t="n">
+        <v>45988.67015928241</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>smart watch</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F78" s="2" t="n">
+        <v>45988.67049449074</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>[Fallback]</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>smart watch</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Sorry, we don’t have that product right now.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F79" s="2" t="n">
+        <v>45988.67072487268</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>[Call Started]</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F80" s="2" t="n">
+        <v>45988.67656203704</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>[Intro response]</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>919510038048</v>
+      </c>
+      <c r="F81" s="2" t="n">
+        <v>45988.67678699074</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>[Product match]</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>laptop</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Laptop Pro  to your phone number ending with 8048. Thank you for your time! I really appreciate it.</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
         <is>
           <t>+919510038048</t>
         </is>
       </c>
-      <c r="F73" s="2" t="n">
-        <v>45987.63049465394</v>
+      <c r="F82" s="2" t="n">
+        <v>45988.67693401646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>